<commit_message>
Update SBA Science Variable Dictionary 2018-2019.xlsx
</commit_message>
<xml_diff>
--- a/SBA Science Variable Dictionary 2018-2019.xlsx
+++ b/SBA Science Variable Dictionary 2018-2019.xlsx
@@ -353,7 +353,7 @@
     <t>3 levels: Online, Paper, Mixed</t>
   </si>
   <si>
-    <t>Last edited on 7/10/2019</t>
+    <t>Last edited on 7/11/2019</t>
   </si>
 </sst>
 </file>
@@ -904,7 +904,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>